<commit_message>
Before trial of the scikit version changing.
</commit_message>
<xml_diff>
--- a/source/math_linreg2/data/calories.xlsx
+++ b/source/math_linreg2/data/calories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>weight</t>
   </si>
@@ -48,6 +48,12 @@
   <si>
     <t>r_errors</t>
   </si>
+  <si>
+    <t>fitted</t>
+  </si>
+  <si>
+    <t>residuals</t>
+  </si>
 </sst>
 </file>
 
@@ -56,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +90,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -152,21 +167,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,15 +491,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:O81"/>
+  <dimension ref="C1:P81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="8" width="8.7265625" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -493,6 +515,12 @@
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
@@ -509,7 +537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C2">
         <v>164</v>
       </c>
@@ -524,6 +552,14 @@
         <f t="shared" ref="F2:F21" si="0">C2*$M$2 +D2*$N$2 +E2*$O$2+I2</f>
         <v>1804.6079999999999</v>
       </c>
+      <c r="G2" s="6">
+        <f>C2*$M$3 +D2*$N$3+E2*$O$3+$P$3</f>
+        <v>1663.2077435217998</v>
+      </c>
+      <c r="H2" s="7">
+        <f>G2-F2</f>
+        <v>-141.40025647820016</v>
+      </c>
       <c r="I2">
         <v>158</v>
       </c>
@@ -543,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C3">
         <v>178</v>
       </c>
@@ -558,14 +594,34 @@
         <f t="shared" si="0"/>
         <v>1882.152</v>
       </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G66" si="2">C3*$M$3 +D3*$N$3+E3*$O$3+$P$3</f>
+        <v>1994.1762700635438</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H66" si="3">G3-F3</f>
+        <v>112.02427006354378</v>
+      </c>
       <c r="I3">
         <v>-137</v>
       </c>
       <c r="J3">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <v>3.8499031499999998</v>
+      </c>
+      <c r="N3">
+        <v>8.9249905100000007</v>
+      </c>
+      <c r="O3">
+        <v>2.1996833699999998</v>
+      </c>
+      <c r="P3">
+        <v>250.94950350079199</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>189</v>
       </c>
@@ -580,6 +636,14 @@
         <f t="shared" si="0"/>
         <v>1853.6990000000001</v>
       </c>
+      <c r="G4" s="6">
+        <f t="shared" si="2"/>
+        <v>1808.6871160054411</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="3"/>
+        <v>-45.011883994558957</v>
+      </c>
       <c r="I4">
         <v>26</v>
       </c>
@@ -594,7 +658,7 @@
         <v>0.39507635579174005</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C5">
         <v>198</v>
       </c>
@@ -609,6 +673,14 @@
         <f t="shared" si="0"/>
         <v>2127.12</v>
       </c>
+      <c r="G5" s="6">
+        <f t="shared" si="2"/>
+        <v>2216.8941469629121</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="3"/>
+        <v>89.774146962912255</v>
+      </c>
       <c r="I5">
         <v>-179</v>
       </c>
@@ -616,7 +688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>189</v>
       </c>
@@ -631,6 +703,14 @@
         <f t="shared" si="0"/>
         <v>2326.4669999999996</v>
       </c>
+      <c r="G6" s="6">
+        <f t="shared" si="2"/>
+        <v>2116.5271856916092</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="3"/>
+        <v>-209.9398143083904</v>
+      </c>
       <c r="I6">
         <v>165</v>
       </c>
@@ -645,7 +725,7 @@
         <v>0.56046462120136442</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>196</v>
       </c>
@@ -660,6 +740,14 @@
         <f t="shared" si="0"/>
         <v>2041.32</v>
       </c>
+      <c r="G7" s="6">
+        <f t="shared" si="2"/>
+        <v>1942.0192959451119</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="3"/>
+        <v>-99.300704054888001</v>
+      </c>
       <c r="I7">
         <v>65</v>
       </c>
@@ -674,7 +762,7 @@
         <v>0.76232151447946372</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C8">
         <v>152</v>
       </c>
@@ -689,6 +777,14 @@
         <f t="shared" si="0"/>
         <v>1744.9119999999998</v>
       </c>
+      <c r="G8" s="6">
+        <f t="shared" si="2"/>
+        <v>1629.0720986413039</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="3"/>
+        <v>-115.8399013586959</v>
+      </c>
       <c r="I8">
         <v>142</v>
       </c>
@@ -703,7 +799,7 @@
         <v>0.13241894652652034</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C9">
         <v>199</v>
       </c>
@@ -718,6 +814,14 @@
         <f t="shared" si="0"/>
         <v>1934.6210000000001</v>
       </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>1999.066670972463</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="3"/>
+        <v>64.445670972462949</v>
+      </c>
       <c r="I9">
         <v>-110</v>
       </c>
@@ -725,7 +829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C10">
         <v>163</v>
       </c>
@@ -740,6 +844,14 @@
         <f t="shared" si="0"/>
         <v>1716.38</v>
       </c>
+      <c r="G10" s="6">
+        <f t="shared" si="2"/>
+        <v>1550.7113659711717</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="3"/>
+        <v>-165.66863402882836</v>
+      </c>
       <c r="I10">
         <v>190</v>
       </c>
@@ -747,7 +859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C11">
         <v>177</v>
       </c>
@@ -762,6 +874,14 @@
         <f t="shared" si="0"/>
         <v>1988.5540000000001</v>
       </c>
+      <c r="G11" s="6">
+        <f t="shared" si="2"/>
+        <v>1936.531137659046</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="3"/>
+        <v>-52.022862340954134</v>
+      </c>
       <c r="I11">
         <v>37</v>
       </c>
@@ -769,7 +889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C12">
         <v>193</v>
       </c>
@@ -784,6 +904,14 @@
         <f t="shared" si="0"/>
         <v>1711.482</v>
       </c>
+      <c r="G12" s="6">
+        <f t="shared" si="2"/>
+        <v>1865.1460980433737</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="3"/>
+        <v>153.66409804337377</v>
+      </c>
       <c r="I12">
         <v>-172</v>
       </c>
@@ -791,7 +919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C13">
         <v>169</v>
       </c>
@@ -806,6 +934,14 @@
         <f t="shared" si="0"/>
         <v>1681.269</v>
       </c>
+      <c r="G13" s="6">
+        <f t="shared" si="2"/>
+        <v>1814.5874185535108</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="3"/>
+        <v>133.31841855351081</v>
+      </c>
       <c r="I13">
         <v>-150</v>
       </c>
@@ -813,7 +949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C14">
         <v>165</v>
       </c>
@@ -828,6 +964,14 @@
         <f t="shared" si="0"/>
         <v>1332.8249999999998</v>
       </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>1486.2274829798669</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="3"/>
+        <v>153.40248297986705</v>
+      </c>
       <c r="I14">
         <v>-125</v>
       </c>
@@ -835,7 +979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C15">
         <v>198</v>
       </c>
@@ -850,6 +994,14 @@
         <f t="shared" si="0"/>
         <v>2116.4880000000003</v>
       </c>
+      <c r="G15" s="6">
+        <f t="shared" si="2"/>
+        <v>1943.5769347096798</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="3"/>
+        <v>-172.91106529032049</v>
+      </c>
       <c r="I15">
         <v>118</v>
       </c>
@@ -857,7 +1009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C16">
         <v>164</v>
       </c>
@@ -872,6 +1024,14 @@
         <f t="shared" si="0"/>
         <v>1724.712</v>
       </c>
+      <c r="G16" s="6">
+        <f t="shared" si="2"/>
+        <v>1582.0113214261037</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="3"/>
+        <v>-142.70067857389631</v>
+      </c>
       <c r="I16">
         <v>157</v>
       </c>
@@ -894,6 +1054,14 @@
         <f t="shared" si="0"/>
         <v>1834.1770000000001</v>
       </c>
+      <c r="G17" s="6">
+        <f t="shared" si="2"/>
+        <v>1706.9643252228188</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="3"/>
+        <v>-127.21267477718129</v>
+      </c>
       <c r="I17">
         <v>107</v>
       </c>
@@ -916,6 +1084,14 @@
         <f t="shared" si="0"/>
         <v>1599.0119999999999</v>
       </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>1785.0301841834039</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="3"/>
+        <v>186.01818418340395</v>
+      </c>
       <c r="I18">
         <v>-185</v>
       </c>
@@ -938,6 +1114,14 @@
         <f t="shared" si="0"/>
         <v>1778.4720000000002</v>
       </c>
+      <c r="G19" s="6">
+        <f t="shared" si="2"/>
+        <v>1811.2580701518641</v>
+      </c>
+      <c r="H19" s="7">
+        <f t="shared" si="3"/>
+        <v>32.786070151863896</v>
+      </c>
       <c r="I19">
         <v>-38</v>
       </c>
@@ -960,6 +1144,14 @@
         <f t="shared" si="0"/>
         <v>1994.836</v>
       </c>
+      <c r="G20" s="6">
+        <f t="shared" si="2"/>
+        <v>1989.4589594454278</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="3"/>
+        <v>-5.3770405545722042</v>
+      </c>
       <c r="I20">
         <v>-26</v>
       </c>
@@ -982,6 +1174,14 @@
         <f t="shared" si="0"/>
         <v>1781.8799999999999</v>
       </c>
+      <c r="G21" s="6">
+        <f t="shared" si="2"/>
+        <v>1866.4352587716719</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="3"/>
+        <v>84.555258771672015</v>
+      </c>
       <c r="I21">
         <v>-85</v>
       </c>
@@ -1001,8 +1201,16 @@
         <v>74</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" ref="F22:F81" si="2">C22*$M$2 +D22*$N$2 +E22*$O$2+I22</f>
+        <f t="shared" ref="F22:F81" si="4">C22*$M$2 +D22*$N$2 +E22*$O$2+I22</f>
         <v>1700.7750000000001</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="2"/>
+        <v>1675.172041839317</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="3"/>
+        <v>-25.602958160683102</v>
       </c>
       <c r="I22">
         <v>33</v>
@@ -1023,8 +1231,16 @@
         <v>92</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2045.692</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="2"/>
+        <v>1994.741870121084</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="3"/>
+        <v>-50.950129878915959</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -1045,8 +1261,16 @@
         <v>102</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1653.692</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="2"/>
+        <v>1604.562476898084</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="3"/>
+        <v>-49.129523101915993</v>
       </c>
       <c r="I24">
         <v>65</v>
@@ -1067,8 +1291,16 @@
         <v>102</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1903.5160000000001</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="2"/>
+        <v>1839.814033677108</v>
+      </c>
+      <c r="H25" s="7">
+        <f t="shared" si="3"/>
+        <v>-63.701966322892076</v>
       </c>
       <c r="I25">
         <v>43</v>
@@ -1089,8 +1321,16 @@
         <v>125</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2156.2840000000001</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="2"/>
+        <v>2022.970937154276</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="3"/>
+        <v>-133.31306284572406</v>
       </c>
       <c r="I26">
         <v>93</v>
@@ -1111,8 +1351,16 @@
         <v>112</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1753</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="2"/>
+        <v>1677.236372865792</v>
+      </c>
+      <c r="H27" s="7">
+        <f t="shared" si="3"/>
+        <v>-75.763627134208036</v>
       </c>
       <c r="I27">
         <v>104</v>
@@ -1133,8 +1381,16 @@
         <v>114</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1807.28</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="2"/>
+        <v>1898.916512802072</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="3"/>
+        <v>91.636512802072048</v>
       </c>
       <c r="I28">
         <v>-118</v>
@@ -1155,8 +1411,16 @@
         <v>98</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2169.8000000000002</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="2"/>
+        <v>1946.3851316255918</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="3"/>
+        <v>-223.41486837440834</v>
       </c>
       <c r="I29">
         <v>199</v>
@@ -1177,8 +1441,16 @@
         <v>87</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1753.0760000000002</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="2"/>
+        <v>1745.2658747296682</v>
+      </c>
+      <c r="H30" s="7">
+        <f t="shared" si="3"/>
+        <v>-7.810125270332037</v>
       </c>
       <c r="I30">
         <v>8</v>
@@ -1199,8 +1471,16 @@
         <v>79</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1797.9359999999999</v>
+      </c>
+      <c r="G31" s="6">
+        <f t="shared" si="2"/>
+        <v>1852.6148973495278</v>
+      </c>
+      <c r="H31" s="7">
+        <f t="shared" si="3"/>
+        <v>54.678897349527915</v>
       </c>
       <c r="I31">
         <v>-78</v>
@@ -1221,8 +1501,16 @@
         <v>110</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1845.0250000000001</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="2"/>
+        <v>1691.1107788750669</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="3"/>
+        <v>-153.91422112493319</v>
       </c>
       <c r="I32">
         <v>172</v>
@@ -1243,8 +1531,16 @@
         <v>108</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1560.8000000000002</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="2"/>
+        <v>1771.4035661195921</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" si="3"/>
+        <v>210.60356611959196</v>
       </c>
       <c r="I33">
         <v>-199</v>
@@ -1265,8 +1561,16 @@
         <v>99</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1500.3440000000001</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="2"/>
+        <v>1698.050972415336</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" si="3"/>
+        <v>197.70697241533594</v>
       </c>
       <c r="I34">
         <v>-189</v>
@@ -1287,8 +1591,16 @@
         <v>115</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1832.989</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="2"/>
+        <v>1919.0759074592308</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" si="3"/>
+        <v>86.086907459230815</v>
       </c>
       <c r="I35">
         <v>-100</v>
@@ -1309,8 +1621,16 @@
         <v>106</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1999.328</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="2"/>
+        <v>2111.6266409545201</v>
+      </c>
+      <c r="H36" s="7">
+        <f t="shared" si="3"/>
+        <v>112.29864095452012</v>
       </c>
       <c r="I36">
         <v>-168</v>
@@ -1331,8 +1651,16 @@
         <v>70</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1905.4479999999999</v>
+      </c>
+      <c r="G37" s="6">
+        <f t="shared" si="2"/>
+        <v>1718.3694576876399</v>
+      </c>
+      <c r="H37" s="7">
+        <f t="shared" si="3"/>
+        <v>-187.07854231236001</v>
       </c>
       <c r="I37">
         <v>173</v>
@@ -1353,8 +1681,16 @@
         <v>109</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1550.9</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="2"/>
+        <v>1612.762763268692</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="3"/>
+        <v>61.862763268691879</v>
       </c>
       <c r="I38">
         <v>-30</v>
@@ -1375,8 +1711,16 @@
         <v>105</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1494.579</v>
+      </c>
+      <c r="G39" s="6">
+        <f t="shared" si="2"/>
+        <v>1636.103426256321</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="3"/>
+        <v>141.52442625632102</v>
       </c>
       <c r="I39">
         <v>-126</v>
@@ -1397,8 +1741,16 @@
         <v>91</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1762.1799999999998</v>
+      </c>
+      <c r="G40" s="6">
+        <f t="shared" si="2"/>
+        <v>1902.291524125972</v>
+      </c>
+      <c r="H40" s="7">
+        <f t="shared" si="3"/>
+        <v>140.11152412597221</v>
       </c>
       <c r="I40">
         <v>-181</v>
@@ -1419,8 +1771,16 @@
         <v>122</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1531.3389999999999</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="2"/>
+        <v>1560.1475771490807</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" si="3"/>
+        <v>28.808577149080747</v>
       </c>
       <c r="I41">
         <v>12</v>
@@ -1441,8 +1801,16 @@
         <v>122</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1970.424</v>
+      </c>
+      <c r="G42" s="6">
+        <f t="shared" si="2"/>
+        <v>1860.3990435314156</v>
+      </c>
+      <c r="H42" s="7">
+        <f t="shared" si="3"/>
+        <v>-110.02495646858438</v>
       </c>
       <c r="I42">
         <v>103</v>
@@ -1463,8 +1831,16 @@
         <v>88</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1567.232</v>
+      </c>
+      <c r="G43" s="6">
+        <f t="shared" si="2"/>
+        <v>1677.340507536624</v>
+      </c>
+      <c r="H43" s="7">
+        <f t="shared" si="3"/>
+        <v>110.10850753662407</v>
       </c>
       <c r="I43">
         <v>-115</v>
@@ -1485,8 +1861,16 @@
         <v>113</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1929.5540000000001</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="2"/>
+        <v>1907.9352538490461</v>
+      </c>
+      <c r="H44" s="7">
+        <f t="shared" si="3"/>
+        <v>-21.618746150953939</v>
       </c>
       <c r="I44">
         <v>4</v>
@@ -1507,8 +1891,16 @@
         <v>100</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1775.4380000000001</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="2"/>
+        <v>1724.60637559313</v>
+      </c>
+      <c r="H45" s="7">
+        <f t="shared" si="3"/>
+        <v>-50.831624406870105</v>
       </c>
       <c r="I45">
         <v>52</v>
@@ -1529,8 +1921,16 @@
         <v>110</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1487.922</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="2"/>
+        <v>1677.6473815888139</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="3"/>
+        <v>189.72538158881389</v>
       </c>
       <c r="I46">
         <v>-181</v>
@@ -1551,8 +1951,16 @@
         <v>88</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1876.348</v>
+      </c>
+      <c r="G47" s="6">
+        <f t="shared" si="2"/>
+        <v>1735.8947173265399</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="3"/>
+        <v>-140.45328267346008</v>
       </c>
       <c r="I47">
         <v>134</v>
@@ -1573,8 +1981,16 @@
         <v>77</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2253.6320000000001</v>
+      </c>
+      <c r="G48" s="6">
+        <f t="shared" si="2"/>
+        <v>2027.3525360300239</v>
+      </c>
+      <c r="H48" s="7">
+        <f t="shared" si="3"/>
+        <v>-226.27946396997618</v>
       </c>
       <c r="I48">
         <v>170</v>
@@ -1595,8 +2011,16 @@
         <v>104</v>
       </c>
       <c r="F49" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1978.7080000000001</v>
+      </c>
+      <c r="G49" s="6">
+        <f t="shared" si="2"/>
+        <v>1905.9671947539</v>
+      </c>
+      <c r="H49" s="7">
+        <f t="shared" si="3"/>
+        <v>-72.740805246100081</v>
       </c>
       <c r="I49">
         <v>45</v>
@@ -1617,8 +2041,16 @@
         <v>106</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1860.3710000000001</v>
+      </c>
+      <c r="G50" s="6">
+        <f t="shared" si="2"/>
+        <v>1900.6497790057128</v>
+      </c>
+      <c r="H50" s="7">
+        <f t="shared" si="3"/>
+        <v>40.278779005712749</v>
       </c>
       <c r="I50">
         <v>-74</v>
@@ -1639,8 +2071,16 @@
         <v>128</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1756.4730000000002</v>
+      </c>
+      <c r="G51" s="6">
+        <f t="shared" si="2"/>
+        <v>1783.007452255915</v>
+      </c>
+      <c r="H51" s="7">
+        <f t="shared" si="3"/>
+        <v>26.534452255914857</v>
       </c>
       <c r="I51">
         <v>-29</v>
@@ -1661,8 +2101,16 @@
         <v>129</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1973</v>
+      </c>
+      <c r="G52" s="6">
+        <f t="shared" si="2"/>
+        <v>1864.4285119657918</v>
+      </c>
+      <c r="H52" s="7">
+        <f t="shared" si="3"/>
+        <v>-108.57148803420819</v>
       </c>
       <c r="I52">
         <v>105</v>
@@ -1683,8 +2131,16 @@
         <v>113</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1605.568</v>
+      </c>
+      <c r="G53" s="6">
+        <f t="shared" si="2"/>
+        <v>1674.72558957876</v>
+      </c>
+      <c r="H53" s="7">
+        <f t="shared" si="3"/>
+        <v>69.157589578760053</v>
       </c>
       <c r="I53">
         <v>-58</v>
@@ -1705,8 +2161,16 @@
         <v>124</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1847.1770000000001</v>
+      </c>
+      <c r="G54" s="6">
+        <f t="shared" si="2"/>
+        <v>1812.5491269828187</v>
+      </c>
+      <c r="H54" s="7">
+        <f t="shared" si="3"/>
+        <v>-34.6278730171814</v>
       </c>
       <c r="I54">
         <v>24</v>
@@ -1727,8 +2191,16 @@
         <v>126</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1914.58</v>
+      </c>
+      <c r="G55" s="6">
+        <f t="shared" si="2"/>
+        <v>1728.3749350183718</v>
+      </c>
+      <c r="H55" s="7">
+        <f t="shared" si="3"/>
+        <v>-186.20506498162808</v>
       </c>
       <c r="I55">
         <v>199</v>
@@ -1749,8 +2221,16 @@
         <v>126</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2458</v>
+      </c>
+      <c r="G56" s="6">
+        <f t="shared" si="2"/>
+        <v>2226.167678853792</v>
+      </c>
+      <c r="H56" s="7">
+        <f t="shared" si="3"/>
+        <v>-231.83232114620796</v>
       </c>
       <c r="I56">
         <v>173</v>
@@ -1771,8 +2251,16 @@
         <v>97</v>
       </c>
       <c r="F57" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1963.95</v>
+      </c>
+      <c r="G57" s="6">
+        <f t="shared" si="2"/>
+        <v>1848.5580335912421</v>
+      </c>
+      <c r="H57" s="7">
+        <f t="shared" si="3"/>
+        <v>-115.39196640875798</v>
       </c>
       <c r="I57">
         <v>92</v>
@@ -1793,8 +2281,16 @@
         <v>129</v>
       </c>
       <c r="F58" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2106.0700000000002</v>
+      </c>
+      <c r="G58" s="6">
+        <f t="shared" si="2"/>
+        <v>2190.9345267133622</v>
+      </c>
+      <c r="H58" s="7">
+        <f t="shared" si="3"/>
+        <v>84.864526713362011</v>
       </c>
       <c r="I58">
         <v>-136</v>
@@ -1815,8 +2311,16 @@
         <v>111</v>
       </c>
       <c r="F59" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1828.0720000000001</v>
+      </c>
+      <c r="G59" s="6">
+        <f t="shared" si="2"/>
+        <v>1682.1353854094641</v>
+      </c>
+      <c r="H59" s="7">
+        <f t="shared" si="3"/>
+        <v>-145.93661459053601</v>
       </c>
       <c r="I59">
         <v>169</v>
@@ -1837,8 +2341,16 @@
         <v>106</v>
       </c>
       <c r="F60" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1581.625</v>
+      </c>
+      <c r="G60" s="6">
+        <f t="shared" si="2"/>
+        <v>1622.506310397667</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="3"/>
+        <v>40.881310397666994</v>
       </c>
       <c r="I60">
         <v>-26</v>
@@ -1859,8 +2371,16 @@
         <v>86</v>
       </c>
       <c r="F61" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2033</v>
+      </c>
+      <c r="G61" s="6">
+        <f t="shared" si="2"/>
+        <v>2138.1803440537919</v>
+      </c>
+      <c r="H61" s="7">
+        <f t="shared" si="3"/>
+        <v>105.18034405379194</v>
       </c>
       <c r="I61">
         <v>-172</v>
@@ -1881,8 +2401,16 @@
         <v>99</v>
       </c>
       <c r="F62" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1844.8</v>
+      </c>
+      <c r="G62" s="6">
+        <f t="shared" si="2"/>
+        <v>1948.5848149955918</v>
+      </c>
+      <c r="H62" s="7">
+        <f t="shared" si="3"/>
+        <v>103.78481499559189</v>
       </c>
       <c r="I62">
         <v>-128</v>
@@ -1903,8 +2431,16 @@
         <v>84</v>
       </c>
       <c r="F63" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1770.7919999999999</v>
+      </c>
+      <c r="G63" s="6">
+        <f t="shared" si="2"/>
+        <v>1861.8053526601839</v>
+      </c>
+      <c r="H63" s="7">
+        <f t="shared" si="3"/>
+        <v>91.013352660183955</v>
       </c>
       <c r="I63">
         <v>-109</v>
@@ -1925,8 +2461,16 @@
         <v>95</v>
       </c>
       <c r="F64" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1955.4740000000002</v>
+      </c>
+      <c r="G64" s="6">
+        <f t="shared" si="2"/>
+        <v>2067.3128575189658</v>
+      </c>
+      <c r="H64" s="7">
+        <f t="shared" si="3"/>
+        <v>111.8388575189656</v>
       </c>
       <c r="I64">
         <v>-168</v>
@@ -1947,8 +2491,16 @@
         <v>124</v>
       </c>
       <c r="F65" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1899.992</v>
+      </c>
+      <c r="G65" s="6">
+        <f t="shared" si="2"/>
+        <v>2009.5735267163839</v>
+      </c>
+      <c r="H65" s="7">
+        <f t="shared" si="3"/>
+        <v>109.58152671638391</v>
       </c>
       <c r="I65">
         <v>-146</v>
@@ -1969,8 +2521,16 @@
         <v>73</v>
       </c>
       <c r="F66" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1798.5749999999998</v>
+      </c>
+      <c r="G66" s="6">
+        <f t="shared" si="2"/>
+        <v>1942.8148612891168</v>
+      </c>
+      <c r="H66" s="7">
+        <f t="shared" si="3"/>
+        <v>144.23986128911702</v>
       </c>
       <c r="I66">
         <v>-197</v>
@@ -1984,15 +2544,23 @@
         <v>190</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" ref="D67:D81" si="3">J67*(C67/100)^2</f>
+        <f t="shared" ref="D67:D81" si="5">J67*(C67/100)^2</f>
         <v>101.08</v>
       </c>
       <c r="E67">
         <v>97</v>
       </c>
       <c r="F67" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2054.8000000000002</v>
+      </c>
+      <c r="G67" s="6">
+        <f t="shared" ref="G67:G81" si="6">C67*$M$3 +D67*$N$3+E67*$O$3+$P$3</f>
+        <v>2097.9384296415919</v>
+      </c>
+      <c r="H67" s="7">
+        <f t="shared" ref="H67:H81" si="7">G67-F67</f>
+        <v>43.138429641591756</v>
       </c>
       <c r="I67">
         <v>-100</v>
@@ -2006,15 +2574,23 @@
         <v>163</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>47.824199999999998</v>
       </c>
       <c r="E68">
         <v>117</v>
       </c>
       <c r="F68" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1681.242</v>
+      </c>
+      <c r="G68" s="6">
+        <f t="shared" si="6"/>
+        <v>1562.677202389134</v>
+      </c>
+      <c r="H68" s="7">
+        <f t="shared" si="7"/>
+        <v>-118.56479761086598</v>
       </c>
       <c r="I68">
         <v>154</v>
@@ -2028,15 +2604,23 @@
         <v>181</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>91.730800000000002</v>
       </c>
       <c r="E69">
         <v>108</v>
       </c>
       <c r="F69" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1851.308</v>
+      </c>
+      <c r="G69" s="6">
+        <f t="shared" si="6"/>
+        <v>2004.0442970855001</v>
+      </c>
+      <c r="H69" s="7">
+        <f t="shared" si="7"/>
+        <v>152.73629708550015</v>
       </c>
       <c r="I69">
         <v>-187</v>
@@ -2050,15 +2634,23 @@
         <v>164</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>51.102399999999989</v>
       </c>
       <c r="E70">
         <v>119</v>
       </c>
       <c r="F70" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1610.0239999999999</v>
+      </c>
+      <c r="G70" s="6">
+        <f t="shared" si="6"/>
+        <v>1600.1843761690159</v>
+      </c>
+      <c r="H70" s="7">
+        <f t="shared" si="7"/>
+        <v>-9.8396238309840101</v>
       </c>
       <c r="I70">
         <v>41</v>
@@ -2072,15 +2664,23 @@
         <v>159</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>70.786799999999999</v>
       </c>
       <c r="E71">
         <v>101</v>
       </c>
       <c r="F71" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1707.8679999999999</v>
+      </c>
+      <c r="G71" s="6">
+        <f t="shared" si="6"/>
+        <v>1717.0236429540601</v>
+      </c>
+      <c r="H71" s="7">
+        <f t="shared" si="7"/>
+        <v>9.155642954060113</v>
       </c>
       <c r="I71">
         <v>3</v>
@@ -2094,15 +2694,23 @@
         <v>160</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>81.920000000000016</v>
       </c>
       <c r="E72">
         <v>74</v>
       </c>
       <c r="F72" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1661.2000000000003</v>
+      </c>
+      <c r="G72" s="6">
+        <f t="shared" si="6"/>
+        <v>1760.8457994599921</v>
+      </c>
+      <c r="H72" s="7">
+        <f t="shared" si="7"/>
+        <v>99.645799459991849</v>
       </c>
       <c r="I72">
         <v>-106</v>
@@ -2116,15 +2724,23 @@
         <v>150</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>56.25</v>
       </c>
       <c r="E73">
         <v>84</v>
       </c>
       <c r="F73" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1595.5</v>
+      </c>
+      <c r="G73" s="6">
+        <f t="shared" si="6"/>
+        <v>1515.239095268292</v>
+      </c>
+      <c r="H73" s="7">
+        <f t="shared" si="7"/>
+        <v>-80.260904731708024</v>
       </c>
       <c r="I73">
         <v>115</v>
@@ -2138,15 +2754,23 @@
         <v>192</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>62.668799999999997</v>
       </c>
       <c r="E74">
         <v>81</v>
       </c>
       <c r="F74" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1606.6880000000001</v>
+      </c>
+      <c r="G74" s="6">
+        <f t="shared" si="6"/>
+        <v>1727.62370654388</v>
+      </c>
+      <c r="H74" s="7">
+        <f t="shared" si="7"/>
+        <v>120.93570654387986</v>
       </c>
       <c r="I74">
         <v>-142</v>
@@ -2160,15 +2784,23 @@
         <v>188</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>77.756799999999998</v>
       </c>
       <c r="E75">
         <v>81</v>
       </c>
       <c r="F75" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1681.568</v>
+      </c>
+      <c r="G75" s="6">
+        <f t="shared" si="6"/>
+        <v>1846.8843507587599</v>
+      </c>
+      <c r="H75" s="7">
+        <f t="shared" si="7"/>
+        <v>165.31635075875988</v>
       </c>
       <c r="I75">
         <v>-198</v>
@@ -2182,15 +2814,23 @@
         <v>162</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>47.239200000000011</v>
       </c>
       <c r="E76">
         <v>71</v>
       </c>
       <c r="F76" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1334.3920000000001</v>
+      </c>
+      <c r="G76" s="6">
+        <f t="shared" si="6"/>
+        <v>1452.420744770784</v>
+      </c>
+      <c r="H76" s="7">
+        <f t="shared" si="7"/>
+        <v>118.02874477078399</v>
       </c>
       <c r="I76">
         <v>-90</v>
@@ -2204,15 +2844,23 @@
         <v>196</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>96.039999999999992</v>
       </c>
       <c r="E77">
         <v>103</v>
       </c>
       <c r="F77" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2237.3999999999996</v>
+      </c>
+      <c r="G77" s="6">
+        <f t="shared" si="6"/>
+        <v>2089.2539965911919</v>
+      </c>
+      <c r="H77" s="7">
+        <f t="shared" si="7"/>
+        <v>-148.1460034088077</v>
       </c>
       <c r="I77">
         <v>91</v>
@@ -2226,15 +2874,23 @@
         <v>174</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>81.745199999999997</v>
       </c>
       <c r="E78">
         <v>77</v>
       </c>
       <c r="F78" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2038.452</v>
+      </c>
+      <c r="G78" s="6">
+        <f t="shared" si="6"/>
+        <v>1819.7834053288439</v>
+      </c>
+      <c r="H78" s="7">
+        <f t="shared" si="7"/>
+        <v>-218.66859467115614</v>
       </c>
       <c r="I78">
         <v>197</v>
@@ -2248,15 +2904,23 @@
         <v>196</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>69.148799999999994</v>
       </c>
       <c r="E79">
         <v>82</v>
       </c>
       <c r="F79" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1959.4879999999998</v>
+      </c>
+      <c r="G79" s="6">
+        <f t="shared" si="6"/>
+        <v>1803.0569410186799</v>
+      </c>
+      <c r="H79" s="7">
+        <f t="shared" si="7"/>
+        <v>-156.43105898131989</v>
       </c>
       <c r="I79">
         <v>124</v>
@@ -2270,15 +2934,23 @@
         <v>176</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>77.44</v>
       </c>
       <c r="E80">
         <v>108</v>
       </c>
       <c r="F80" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1681.4</v>
+      </c>
+      <c r="G80" s="6">
+        <f t="shared" si="6"/>
+        <v>1857.2495269551919</v>
+      </c>
+      <c r="H80" s="7">
+        <f t="shared" si="7"/>
+        <v>175.84952695519178</v>
       </c>
       <c r="I80">
         <v>-189</v>
@@ -2292,15 +2964,23 @@
         <v>166</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>57.867599999999996</v>
       </c>
       <c r="E81">
         <v>122</v>
       </c>
       <c r="F81" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1497.6759999999999</v>
+      </c>
+      <c r="G81" s="6">
+        <f t="shared" si="6"/>
+        <v>1674.8625783772679</v>
+      </c>
+      <c r="H81" s="7">
+        <f t="shared" si="7"/>
+        <v>177.18657837726801</v>
       </c>
       <c r="I81">
         <v>-155</v>

</xml_diff>